<commit_message>
Fix local schedule test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/example_2.xlsx
+++ b/cypress/fixtures/example_2.xlsx
@@ -202,9 +202,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -212,6 +209,9 @@
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,17 +1284,17 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>10</v>
@@ -1308,82 +1308,82 @@
       <c r="J6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="K6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="R6" s="4" t="s">
+      <c r="O6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="3" t="s">
+      <c r="S6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE6" s="3" t="s">
+      <c r="W6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AF6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG6" s="5" t="s">
+      <c r="AF6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AH6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1391,109 +1391,109 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="5" t="s">
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF7" s="4" t="s">
+      <c r="T7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AG7" s="5" t="s">
+      <c r="AG7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AH7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI7" s="3" t="s">
+      <c r="AH7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AJ7" s="3" t="s">
+      <c r="AJ7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1507,10 +1507,10 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1528,82 +1528,82 @@
       <c r="J8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="L8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="N8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="4" t="s">
+      <c r="P8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U8" s="3" t="s">
+      <c r="S8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="X8" s="3" t="s">
+      <c r="V8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB8" s="3" t="s">
+      <c r="Y8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AC8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
+      <c r="AC8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1629,82 +1629,82 @@
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AE9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AF9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG9" s="5" t="s">
+      <c r="AF9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AH9" s="6" t="s">
@@ -1721,109 +1721,109 @@
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T10" s="3" t="s">
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W10" s="3" t="s">
+      <c r="U10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE10" s="3" t="s">
+      <c r="X10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AF10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG10" s="5" t="s">
+      <c r="AF10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AH10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI10" s="3" t="s">
+      <c r="AH10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AJ10" s="3" t="s">
+      <c r="AJ10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1831,16 +1831,16 @@
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1858,10 +1858,10 @@
       <c r="J11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="6" t="s">
@@ -1879,10 +1879,10 @@
       <c r="Q11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S11" s="5" t="s">
+      <c r="R11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="T11" s="6" t="s">
@@ -1900,40 +1900,40 @@
       <c r="X11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD11" s="3" t="s">
+      <c r="Y11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AE11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG11" s="5" t="s">
+      <c r="AE11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
+      <c r="AH11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1947,31 +1947,31 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5" t="s">
+      <c r="K12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="6" t="s">
@@ -1989,10 +1989,10 @@
       <c r="Q12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="5" t="s">
+      <c r="R12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="T12" s="6" t="s">
@@ -2010,40 +2010,40 @@
       <c r="X12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ12" s="3" t="s">
+      <c r="Y12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2057,103 +2057,103 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE13" s="3" t="s">
+      <c r="R13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AF13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ13" s="3" t="s">
+      <c r="AF13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2161,16 +2161,16 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -2188,82 +2188,82 @@
       <c r="J14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="5" t="s">
+      <c r="K14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="3" t="s">
+      <c r="M14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q14" s="3" t="s">
+      <c r="O14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X14" s="3" t="s">
+      <c r="R14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC14" s="3" t="s">
+      <c r="Y14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE14" s="3" t="s">
+      <c r="AD14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AF14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG14" s="5" t="s">
+      <c r="AF14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
+      <c r="AH14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2573,37 +2573,37 @@
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="K16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="6" t="s">
@@ -2621,10 +2621,10 @@
       <c r="Q16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="5" t="s">
+      <c r="R16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="T16" s="6" t="s">
@@ -2639,43 +2639,43 @@
       <c r="W16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="X16" s="3" t="s">
+      <c r="X16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ16" s="3" t="s">
+      <c r="Y16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2689,31 +2689,31 @@
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="5" t="s">
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="7" t="s">
@@ -2731,10 +2731,10 @@
       <c r="Q17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S17" s="5" t="s">
+      <c r="R17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T17" s="7" t="s">
@@ -2752,10 +2752,10 @@
       <c r="X17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z17" s="5" t="s">
+      <c r="Y17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AA17" s="7" t="s">
@@ -2773,10 +2773,10 @@
       <c r="AE17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AF17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG17" s="5" t="s">
+      <c r="AF17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AH17" s="7" t="s">
@@ -2799,31 +2799,31 @@
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="3" t="s">
+      <c r="F18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="K18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="6" t="s">
@@ -2841,10 +2841,10 @@
       <c r="Q18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S18" s="5" t="s">
+      <c r="R18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="T18" s="6" t="s">
@@ -2862,40 +2862,40 @@
       <c r="X18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z18" s="5" t="s">
+      <c r="Y18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AA18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AB18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF18" s="4" t="s">
+      <c r="AB18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AG18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI18" s="3" t="s">
+      <c r="AG18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AJ18" s="3" t="s">
+      <c r="AJ18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2909,103 +2909,103 @@
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S19" s="5" t="s">
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="X19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA19" s="3" t="s">
+      <c r="T19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AB19" s="3" t="s">
+      <c r="AB19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF19" s="4" t="s">
+      <c r="AC19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AG19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ19" s="3" t="s">
+      <c r="AG19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3013,109 +3013,109 @@
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="3" t="s">
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="V20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC20" s="3" t="s">
+      <c r="O20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AD20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI20" s="3" t="s">
+      <c r="AD20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AJ20" s="3" t="s">
+      <c r="AJ20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3129,103 +3129,103 @@
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V21" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="W21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD21" s="3" t="s">
+      <c r="W21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AE21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ21" s="3" t="s">
+      <c r="AE21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3245,55 +3245,55 @@
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L22" s="5" t="s">
+      <c r="F22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="R22" s="4" t="s">
+      <c r="M22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U22" s="3" t="s">
+      <c r="S22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V22" s="3" t="s">
+      <c r="V22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W22" s="6" t="s">
@@ -3302,10 +3302,10 @@
       <c r="X22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z22" s="5" t="s">
+      <c r="Y22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AA22" s="6" t="s">
@@ -3323,10 +3323,10 @@
       <c r="AE22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AF22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG22" s="5" t="s">
+      <c r="AF22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AH22" s="6" t="s">
@@ -3349,10 +3349,10 @@
       <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="7" t="s">
@@ -3370,10 +3370,10 @@
       <c r="J23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="5" t="s">
+      <c r="K23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="M23" s="7" t="s">
@@ -3391,10 +3391,10 @@
       <c r="Q23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S23" s="5" t="s">
+      <c r="R23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T23" s="7" t="s">
@@ -3412,10 +3412,10 @@
       <c r="X23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z23" s="5" t="s">
+      <c r="Y23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AA23" s="7" t="s">
@@ -3433,10 +3433,10 @@
       <c r="AE23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AF23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG23" s="5" t="s">
+      <c r="AF23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AH23" s="7" t="s">
@@ -3465,88 +3465,88 @@
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q24" s="3" t="s">
+      <c r="F24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W24" s="3" t="s">
+      <c r="R24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD24" s="3" t="s">
+      <c r="X24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AE24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AF24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG24" s="5" t="s">
+      <c r="AF24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AH24" s="6" t="s">
@@ -3578,46 +3578,46 @@
       <c r="F25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="S25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T25" s="3" t="s">
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="U25" s="7" t="s">
@@ -3632,10 +3632,10 @@
       <c r="X25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z25" s="5" t="s">
+      <c r="Y25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AA25" s="7" t="s">
@@ -3653,10 +3653,10 @@
       <c r="AE25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AF25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG25" s="5" t="s">
+      <c r="AF25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AH25" s="7" t="s">

</xml_diff>